<commit_message>
new spreadsheet with tweet similarity info
</commit_message>
<xml_diff>
--- a/twitter_data/more_rt_fav_analysis.xlsx
+++ b/twitter_data/more_rt_fav_analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="60" windowWidth="11580" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="4500" yWindow="6120" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,11 +387,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2113225496"/>
-        <c:axId val="2113380312"/>
+        <c:axId val="-2116546952"/>
+        <c:axId val="-2116550040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2113225496"/>
+        <c:axId val="-2116546952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -400,7 +400,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113380312"/>
+        <c:crossAx val="-2116550040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -408,7 +408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113380312"/>
+        <c:axId val="-2116550040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -419,7 +419,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113225496"/>
+        <c:crossAx val="-2116546952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -621,11 +621,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2126557544"/>
-        <c:axId val="2117688728"/>
+        <c:axId val="-2116587944"/>
+        <c:axId val="-2116595352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126557544"/>
+        <c:axId val="-2116587944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -634,7 +634,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117688728"/>
+        <c:crossAx val="-2116595352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -642,7 +642,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117688728"/>
+        <c:axId val="-2116595352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,7 +653,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126557544"/>
+        <c:crossAx val="-2116587944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1064,7 +1064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>

</xml_diff>